<commit_message>
Recalculated integral gains from manual tuning to fit Ziegler Nichols proportions, better than actual Ziegler Nichols since there is no real ultimate gain
</commit_message>
<xml_diff>
--- a/zieglerNichols.xlsx
+++ b/zieglerNichols.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Documents\Navales\Master\Q3\Mechatronics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Documents\Navales\Master\Q3\Mechatronics\mechatronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="10">
   <si>
     <t>Ku</t>
   </si>
@@ -48,14 +48,28 @@
   </si>
   <si>
     <t>Yaw</t>
+  </si>
+  <si>
+    <t>Direct Ziegler Nichols, but there is no real Ku</t>
+  </si>
+  <si>
+    <t>Ki from our Kp and Kd with Ziegler Nichols proportions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +97,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,135 +381,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>11.6</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>18.2</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>5.7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <f>0.6*B2</f>
-        <v>7.1999999999999993</v>
+        <v>11.6</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <f>0.6*E2</f>
-        <v>6</v>
+        <v>18.2</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <f>0.6*H2</f>
-        <v>3.5999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <f>1.2*B2/B3</f>
-        <v>1.2413793103448274</v>
+        <f>0.6*B3</f>
+        <v>7.1999999999999993</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5">
-        <f>1.2*E2/E3</f>
-        <v>0.65934065934065933</v>
+        <f>0.6*E3</f>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <f>1.2*H2/H3</f>
-        <v>1.263157894736842</v>
+        <f>0.6*H3</f>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f>1.2*B3/B4</f>
+        <v>1.2413793103448274</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>1.2*E3/E4</f>
+        <v>0.65934065934065933</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <f>1.2*H3/H4</f>
+        <v>1.263157894736842</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <f>0.075*B2*B3</f>
+      <c r="B7">
+        <f>0.075*B3*B4</f>
         <v>10.44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E6">
-        <f>0.075*E2*E3</f>
+      <c r="E7">
+        <f>0.075*E3*E4</f>
         <v>13.649999999999999</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>5</v>
       </c>
-      <c r="H6">
-        <f>0.075*H2*H3</f>
+      <c r="H7">
+        <f>0.075*H3*H4</f>
         <v>2.5649999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>10.59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>55.72</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>49.6</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>225.8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>8.66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <f>B11/0.6</f>
+        <v>17.650000000000002</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>E11/0.6</f>
+        <v>92.866666666666674</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f>H11/0.6</f>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <f>B12/0.075/B14</f>
+        <v>37.469310670443811</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f>E12/0.075/E14</f>
+        <v>32.419239052404883</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <f>H12/0.075/H14</f>
+        <v>26.242424242424242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <f>1.2*B14/B15</f>
+        <v>0.56526260080645174</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <f>1.2*E14/E15</f>
+        <v>3.437465013286094</v>
+      </c>
+      <c r="G16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="2">
+        <f>1.2*H14/H15</f>
+        <v>0.20120092378752888</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>